<commit_message>
- excel: formatNumber 2 digit
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoHangHoaNhapXuatTon.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoHangHoaNhapXuatTon.xlsx
@@ -219,24 +219,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -254,6 +242,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -564,7 +564,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,105 +574,105 @@
     <col min="3" max="3" width="34.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" style="4" customWidth="1"/>
     <col min="5" max="7" width="23" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="7" customWidth="1"/>
-    <col min="12" max="15" width="18" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="14" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="14" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="14" customWidth="1"/>
+    <col min="12" max="15" width="18" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="14" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:17" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -684,15 +684,15 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -702,15 +702,15 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -720,15 +720,15 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -738,15 +738,15 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -756,15 +756,15 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -774,15 +774,15 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -792,15 +792,15 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -810,15 +810,15 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -828,15 +828,15 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -846,15 +846,15 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -864,15 +864,15 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -882,15 +882,15 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -900,15 +900,15 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -918,15 +918,15 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -936,15 +936,15 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
@@ -954,15 +954,15 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -972,15 +972,15 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -990,15 +990,15 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1008,15 +1008,15 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1026,15 +1026,15 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
@@ -1044,15 +1044,15 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -1062,15 +1062,15 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
@@ -1080,15 +1080,15 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -1098,59 +1098,59 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
     </row>
     <row r="29" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="8">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="17">
         <f>SUM(H$5:H28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="17">
         <f>SUM(I$5:I28)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="17">
         <f>SUM(J$5:J28)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="17">
         <f>SUM(K$5:K28)</f>
         <v>0</v>
       </c>
-      <c r="L29" s="8">
+      <c r="L29" s="17">
         <f>SUM(L$5:L28)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="8">
+      <c r="M29" s="17">
         <f>SUM(M$5:M28)</f>
         <v>0</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="17">
         <f>SUM(N$5:N28)</f>
         <v>0</v>
       </c>
-      <c r="O29" s="8">
+      <c r="O29" s="17">
         <f>SUM(O$5:O28)</f>
         <v>0</v>
       </c>
-      <c r="P29" s="8">
+      <c r="P29" s="17">
         <f>SUM(P$5:P28)</f>
         <v>0</v>
       </c>

</xml_diff>